<commit_message>
my sql db services
</commit_message>
<xml_diff>
--- a/pogoda.xlsx
+++ b/pogoda.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,222 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>18.05</v>
+      </c>
+      <c r="B7" t="n">
+        <v>17.79</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D7" t="n">
+        <v>72</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>17:04:16 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>18.05</v>
+      </c>
+      <c r="B8" t="n">
+        <v>17.79</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D8" t="n">
+        <v>72</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>17:04:29 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>18.05</v>
+      </c>
+      <c r="B9" t="n">
+        <v>17.79</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D9" t="n">
+        <v>72</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>17:08:06 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>18.05</v>
+      </c>
+      <c r="B10" t="n">
+        <v>17.79</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D10" t="n">
+        <v>72</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>17:08:18 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>18.27</v>
+      </c>
+      <c r="B11" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D11" t="n">
+        <v>70</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>17:25:33 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>18.27</v>
+      </c>
+      <c r="B12" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>17:25:56 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>17.93</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D13" t="n">
+        <v>71</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>17:40:59 15/11/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="B14" t="n">
+        <v>17.93</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D14" t="n">
+        <v>71</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Lisbon</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>17:41:11 15/11/2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>